<commit_message>
table row added to excel
</commit_message>
<xml_diff>
--- a/public/export.xlsx
+++ b/public/export.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -31,7 +31,7 @@
     <t>DATE</t>
   </si>
   <si>
-    <t>04/27/2021</t>
+    <t>04/28/2021</t>
   </si>
   <si>
     <t>CONTRACT NO.</t>
@@ -55,19 +55,19 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t>07:25:00</t>
+    <t>07:00:00</t>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
-    <t>Partly Cloudy</t>
+    <t/>
   </si>
   <si>
     <t xml:space="preserve">END TIME </t>
   </si>
   <si>
-    <t>18:28:00</t>
+    <t>17:50:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -90,6 +90,21 @@
   <si>
     <t xml:space="preserve">HOURS
 /Day</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>test3</t>
+  </si>
+  <si>
+    <t>tes3</t>
+  </si>
+  <si>
+    <t>test4</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -1440,40 +1455,88 @@
       <c r="G7" s="39"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="43"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="45"/>
+      <c r="A8" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="42">
+        <v>1</v>
+      </c>
+      <c r="D8" s="43">
+        <v>1</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>24</v>
+      </c>
       <c r="G8" s="46"/>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="47"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="49"/>
-      <c r="D9" s="50"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="52"/>
+      <c r="A9" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="49">
+        <v>4</v>
+      </c>
+      <c r="D9" s="50">
+        <v>4</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>24</v>
+      </c>
       <c r="G9" s="53"/>
       <c r="M9" s="54"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="47"/>
-      <c r="B10" s="48"/>
-      <c r="C10" s="49"/>
-      <c r="D10" s="50"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="52"/>
+      <c r="A10" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="48" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="49">
+        <v>12</v>
+      </c>
+      <c r="D10" s="50">
+        <v>0</v>
+      </c>
+      <c r="E10" s="51" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="52" t="s">
+        <v>26</v>
+      </c>
       <c r="G10" s="53"/>
     </row>
     <row r="11" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="49"/>
-      <c r="D11" s="50"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="52"/>
+      <c r="A11" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="49">
+        <v>3</v>
+      </c>
+      <c r="D11" s="50">
+        <v>0</v>
+      </c>
+      <c r="E11" s="51" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="52" t="s">
+        <v>14</v>
+      </c>
       <c r="G11" s="53"/>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1514,7 +1577,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B16" s="56"/>
       <c r="C16" s="57">
@@ -1531,7 +1594,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B17" s="64"/>
       <c r="C17" s="64"/>
@@ -1542,7 +1605,9 @@
       <c r="N17" s="1"/>
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
+      <c r="A18" s="66" t="s">
+        <v>14</v>
+      </c>
       <c r="B18" s="67"/>
       <c r="C18" s="67"/>
       <c r="D18" s="67"/>
@@ -1581,7 +1646,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B22" s="64"/>
       <c r="C22" s="64"/>
@@ -1592,7 +1657,9 @@
       <c r="N22" s="1"/>
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="66"/>
+      <c r="A23" s="66" t="s">
+        <v>14</v>
+      </c>
       <c r="B23" s="67"/>
       <c r="C23" s="67"/>
       <c r="D23" s="67"/>
@@ -1630,7 +1697,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
@@ -1641,7 +1708,9 @@
       <c r="N27" s="1"/>
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="66" t="s">
+        <v>14</v>
+      </c>
       <c r="B28" s="67"/>
       <c r="C28" s="67"/>
       <c r="D28" s="67"/>

</xml_diff>

<commit_message>
unique excelfile name set
</commit_message>
<xml_diff>
--- a/public/export.xlsx
+++ b/public/export.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>DAILY REPORT</t>
   </si>
@@ -25,7 +25,7 @@
     <t>PROJECT NAME</t>
   </si>
   <si>
-    <t>Test Name</t>
+    <t>Health Center - Icardo Plaza ADA Improvements and Road Repairs</t>
   </si>
   <si>
     <t>DATE</t>
@@ -43,7 +43,7 @@
     <t xml:space="preserve">PROJECT ID </t>
   </si>
   <si>
-    <t>999999</t>
+    <t>6141</t>
   </si>
   <si>
     <t xml:space="preserve">DOCUMENTED BY </t>
@@ -55,19 +55,13 @@
     <t xml:space="preserve">START TIME </t>
   </si>
   <si>
-    <t>07:00:00</t>
+    <t/>
   </si>
   <si>
     <t>WEATHER</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t xml:space="preserve">END TIME </t>
-  </si>
-  <si>
-    <t>17:50:00</t>
   </si>
   <si>
     <t>CONTRACTOR</t>
@@ -90,21 +84,6 @@
   <si>
     <t xml:space="preserve">HOURS
 /Day</t>
-  </si>
-  <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>tes3</t>
-  </si>
-  <si>
-    <t>test4</t>
   </si>
   <si>
     <t>TOTAL</t>
@@ -1410,34 +1389,34 @@
         <v>13</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5" s="24"/>
       <c r="D5" s="25"/>
       <c r="E5" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G5" s="22"/>
     </row>
     <row r="6" ht="19.5" customHeight="1" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="29" t="s">
         <v>17</v>
-      </c>
-      <c r="B6" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>19</v>
       </c>
       <c r="D6" s="30"/>
       <c r="E6" s="31" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G6" s="33"/>
     </row>
@@ -1445,98 +1424,50 @@
       <c r="A7" s="15"/>
       <c r="B7" s="34"/>
       <c r="C7" s="35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D7" s="36" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E7" s="37"/>
       <c r="F7" s="38"/>
       <c r="G7" s="39"/>
     </row>
     <row r="8" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="41" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="42">
-        <v>1</v>
-      </c>
-      <c r="D8" s="43">
-        <v>1</v>
-      </c>
-      <c r="E8" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="F8" s="45" t="s">
-        <v>24</v>
-      </c>
+      <c r="A8" s="40"/>
+      <c r="B8" s="41"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="45"/>
       <c r="G8" s="46"/>
     </row>
     <row r="9" ht="19.5" customHeight="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="47" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="48" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="49">
-        <v>4</v>
-      </c>
-      <c r="D9" s="50">
-        <v>4</v>
-      </c>
-      <c r="E9" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="F9" s="52" t="s">
-        <v>24</v>
-      </c>
+      <c r="A9" s="47"/>
+      <c r="B9" s="48"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51"/>
+      <c r="F9" s="52"/>
       <c r="G9" s="53"/>
       <c r="M9" s="54"/>
     </row>
     <row r="10" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="49">
-        <v>12</v>
-      </c>
-      <c r="D10" s="50">
-        <v>0</v>
-      </c>
-      <c r="E10" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="F10" s="52" t="s">
-        <v>26</v>
-      </c>
+      <c r="A10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51"/>
+      <c r="F10" s="52"/>
       <c r="G10" s="53"/>
     </row>
     <row r="11" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="C11" s="49">
-        <v>3</v>
-      </c>
-      <c r="D11" s="50">
-        <v>0</v>
-      </c>
-      <c r="E11" s="51" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="52" t="s">
-        <v>14</v>
-      </c>
+      <c r="A11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51"/>
+      <c r="F11" s="52"/>
       <c r="G11" s="53"/>
     </row>
     <row r="12" ht="19.5" customHeight="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1577,7 +1508,7 @@
     </row>
     <row r="16" ht="24.75" customHeight="1" spans="1:16" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B16" s="56"/>
       <c r="C16" s="57">
@@ -1594,7 +1525,7 @@
     </row>
     <row r="17" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="63" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B17" s="64"/>
       <c r="C17" s="64"/>
@@ -1606,7 +1537,7 @@
     </row>
     <row r="18" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B18" s="67"/>
       <c r="C18" s="67"/>
@@ -1646,7 +1577,7 @@
     </row>
     <row r="22" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="63" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="B22" s="64"/>
       <c r="C22" s="64"/>
@@ -1658,7 +1589,7 @@
     </row>
     <row r="23" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B23" s="67"/>
       <c r="C23" s="67"/>
@@ -1697,7 +1628,7 @@
     </row>
     <row r="27" ht="23.25" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="63" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="B27" s="64"/>
       <c r="C27" s="64"/>
@@ -1709,7 +1640,7 @@
     </row>
     <row r="28" ht="18" customHeight="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="66" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B28" s="67"/>
       <c r="C28" s="67"/>

</xml_diff>